<commit_message>
[experiments][suricataV2] bm, bigFlows, 1x, update title.
</commit_message>
<xml_diff>
--- a/experiments/suricata_with_stat/data/bm,bigFlows,1,1,tcpreplay.xlsx
+++ b/experiments/suricata_with_stat/data/bm,bigFlows,1,1,tcpreplay.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20160405.222455" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Packets sent by 1x TCPreplay</a:t>
+              <a:t>Packets sent to by 1x TCPreplay (Bare metal)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1816,7 +1816,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Traffic sent by 1x TCPreplay </a:t>
+              <a:t>Traffic sent by 1x TCPreplay (Bare metal) </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9480,8 +9480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11336,8 +11336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[experiments][suricataV2] bm, bigFlows, 1x, resize graph.
</commit_message>
<xml_diff>
--- a/experiments/suricata_with_stat/data/bm,bigFlows,1,1,tcpreplay.xlsx
+++ b/experiments/suricata_with_stat/data/bm,bigFlows,1,1,tcpreplay.xlsx
@@ -1776,7 +1776,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2966,7 +2966,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4094,16 +4094,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>407988</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4129,16 +4129,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>80962</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9481,7 +9481,7 @@
   <dimension ref="A1:C251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11337,7 +11337,7 @@
   <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[experiments][suricataV2] bm, bigFlows, 1x & 2x.
</commit_message>
<xml_diff>
--- a/experiments/suricata_with_stat/data/bm,bigFlows,1,1,tcpreplay.xlsx
+++ b/experiments/suricata_with_stat/data/bm,bigFlows,1,1,tcpreplay.xlsx
@@ -233,7 +233,7 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
+      <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -251,14 +251,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>PktT!$A$3:$A$62</c:f>
@@ -637,6 +640,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -653,14 +657,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>PktT!$A$3:$A$62</c:f>
@@ -1039,6 +1046,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1048,11 +1056,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47732528"/>
-        <c:axId val="47733088"/>
+        <c:smooth val="0"/>
+        <c:axId val="415631472"/>
+        <c:axId val="415635392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredAreaSeries>
+            <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="0"/>
                 <c:order val="0"/>
@@ -1074,14 +1083,17 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent6"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
                   </a:ln>
                   <a:effectLst/>
                 </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
                 <c:cat>
                   <c:numRef>
                     <c:extLst>
@@ -1472,13 +1484,14 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
+                <c:smooth val="1"/>
               </c15:ser>
-            </c15:filteredAreaSeries>
+            </c15:filteredLineSeries>
           </c:ext>
         </c:extLst>
-      </c:areaChart>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="47732528"/>
+        <c:axId val="415631472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47733088"/>
+        <c:crossAx val="415635392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47733088"/>
+        <c:axId val="415635392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1697,9 +1710,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47732528"/>
+        <c:crossAx val="415631472"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1854,7 +1867,7 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
+      <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -1872,14 +1885,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>BytesT!$A$3:$A$62</c:f>
@@ -2258,6 +2274,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2274,14 +2291,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>BytesT!$A$3:$A$62</c:f>
@@ -2660,6 +2680,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2669,11 +2690,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371909664"/>
-        <c:axId val="371907424"/>
-      </c:areaChart>
+        <c:smooth val="0"/>
+        <c:axId val="137675072"/>
+        <c:axId val="137677312"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="371909664"/>
+        <c:axId val="137675072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,7 +2794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371907424"/>
+        <c:crossAx val="137677312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2780,7 +2802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="371907424"/>
+        <c:axId val="137677312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2887,9 +2909,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371909664"/>
+        <c:crossAx val="137675072"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9481,7 +9503,7 @@
   <dimension ref="A1:C251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11337,7 +11359,7 @@
   <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>